<commit_message>
add working chatbot + Gemini + Excel save
</commit_message>
<xml_diff>
--- a/data/chat_history.xlsx
+++ b/data/chat_history.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\travel ai\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBE828E-D88B-4615-90AF-F9DB816EA677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB634454-9ECF-4E8D-B066-FF5CCF29210F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,13 +27,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>timestamp</t>
+    <t>session_id</t>
   </si>
   <si>
-    <t xml:space="preserve">	user_input</t>
+    <t>role</t>
   </si>
   <si>
-    <t>ai_response</t>
+    <t>message</t>
   </si>
 </sst>
 </file>
@@ -354,7 +354,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>